<commit_message>
convert dict to excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,188 +425,188 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Etymology 1</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Etymology 2</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>inh From 0</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Pronunciation</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Verb</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>Adjective</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>inh From 0</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>Pronunciation</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>Verb</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>Adverb</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>ar</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>translation</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>transliteration</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>pron_text</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>Audio</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="1" t="inlineStr">
         <is>
           <t>fr</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="1" t="inlineStr">
         <is>
           <t>translation</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" s="1" t="inlineStr">
         <is>
           <t>transliteration</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" s="1" t="inlineStr">
         <is>
           <t>pron_text</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>Audio</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P3" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R3" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>ary</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>meaning</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>meaning</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>ary</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" s="1" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="P4" s="1" t="inlineStr">
         <is>
           <t>meaning</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" s="1" t="inlineStr">
         <is>
           <t>meaning</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" s="1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
@@ -733,6 +736,44 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="M3"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="D3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G4"/>
+    <mergeCell ref="I4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="S4"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3"/>
+    <mergeCell ref="C3"/>
+    <mergeCell ref="F4"/>
+    <mergeCell ref="O3"/>
+    <mergeCell ref="E3"/>
+    <mergeCell ref="N4"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P4"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="B3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="H4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="R4"/>
+    <mergeCell ref="E4"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N3"/>
+    <mergeCell ref="F3"/>
+    <mergeCell ref="L3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="O4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="Q4"/>
+    <mergeCell ref="J4"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>